<commit_message>
orders 수정, rma 추가
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\aristaOrder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E814FD-B372-45B9-A486-CA38D20F49B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41474B6-36AA-42FD-A1F7-59F95A0EA85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="1440" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ORDERS" sheetId="1" r:id="rId1"/>
     <sheet name="ITEMS" sheetId="2" r:id="rId2"/>
+    <sheet name="ETC ORDERS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>CUSTOMER PO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -544,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE8816D-3930-46CC-ABD7-A14746CC51EC}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -601,4 +602,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F092BBF-D8BE-4C21-8366-A520468B8627}">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.625" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>